<commit_message>
Save into param variable
</commit_message>
<xml_diff>
--- a/test/test238b.xlsx
+++ b/test/test238b.xlsx
@@ -383,10 +383,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B2">
         <v>2</v>
       </c>
     </row>

</xml_diff>